<commit_message>
updated schema for one to one relationships for user
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F51E6D-6249-471B-ABF2-0D809196C4C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED5AC90-6D63-41C3-84C0-CEAC42596D06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="540" windowWidth="22545" windowHeight="14355" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="30765" yWindow="975" windowWidth="22545" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="172">
   <si>
     <t>Questionaire</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Authentication</t>
   </si>
   <si>
-    <t>UUID</t>
-  </si>
-  <si>
     <t>Race</t>
   </si>
   <si>
@@ -466,9 +463,6 @@
     <t>List</t>
   </si>
   <si>
-    <t>USER UUID</t>
-  </si>
-  <si>
     <t>Main DB</t>
   </si>
   <si>
@@ -490,9 +484,6 @@
     <t>Profile Table</t>
   </si>
   <si>
-    <t>UUID Table</t>
-  </si>
-  <si>
     <t>Team Workflow Planning Framework</t>
   </si>
   <si>
@@ -548,6 +539,18 @@
   </si>
   <si>
     <t>zip code</t>
+  </si>
+  <si>
+    <t>Amplify</t>
+  </si>
+  <si>
+    <t>Userdb</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>uername</t>
   </si>
 </sst>
 </file>
@@ -1782,19 +1785,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -2709,59 +2700,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2567FF76-5979-4C99-80B2-48D71BE83D83}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1914525" y="361951"/>
-          <a:ext cx="1666875" cy="1752599"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>7</xdr:row>
@@ -2947,6 +2885,59 @@
         <a:xfrm>
           <a:off x="1905000" y="2314575"/>
           <a:ext cx="1752600" cy="3514725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D932F873-D35E-4305-AC44-1C84627838E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1828800" y="304800"/>
+          <a:ext cx="1838325" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3277,8 +3268,8 @@
   </sheetPr>
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3294,80 +3285,80 @@
   <sheetData>
     <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="E1" s="80" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E2" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D4" s="128" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E4" s="128" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F4" s="128" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D5" s="128" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E5" s="128"/>
       <c r="F5" s="128" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="141"/>
       <c r="C6" s="142"/>
       <c r="D6" s="143" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="143" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="143" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="143" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="143" t="s">
-        <v>89</v>
-      </c>
       <c r="G6" s="143" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H6" s="144" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="138" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="129" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" s="129" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" s="145" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H7" s="137" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="139"/>
       <c r="C8" s="129" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D8" s="130"/>
       <c r="E8" s="130"/>
@@ -3383,24 +3374,24 @@
       </c>
       <c r="J8" s="1">
         <f ca="1">TODAY()</f>
-        <v>44292</v>
+        <v>44293</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="120" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="76" t="s">
         <v>97</v>
-      </c>
-      <c r="D9" s="75" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="75" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="76" t="s">
-        <v>98</v>
       </c>
       <c r="G9" s="157">
         <v>44292</v>
@@ -3416,16 +3407,16 @@
     <row r="10" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="121"/>
       <c r="C10" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="78" t="s">
+      <c r="E10" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="79" t="s">
         <v>93</v>
-      </c>
-      <c r="E10" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="79" t="s">
-        <v>94</v>
       </c>
       <c r="G10" s="157">
         <v>44292</v>
@@ -3441,16 +3432,16 @@
     <row r="11" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="122"/>
       <c r="C11" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="75" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="82" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="2">
         <v>44296</v>
@@ -3463,19 +3454,19 @@
     </row>
     <row r="12" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="83" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="84" t="s">
         <v>107</v>
-      </c>
-      <c r="F12" s="84" t="s">
-        <v>108</v>
       </c>
       <c r="G12" s="2">
         <v>44296</v>
@@ -3489,16 +3480,16 @@
     <row r="13" spans="2:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="124"/>
       <c r="C13" s="85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="86" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" s="2">
         <v>44296</v>
@@ -3512,10 +3503,10 @@
     <row r="14" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="125"/>
       <c r="C14" s="93" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="94" t="s">
         <v>113</v>
-      </c>
-      <c r="D14" s="94" t="s">
-        <v>114</v>
       </c>
       <c r="E14" s="95"/>
       <c r="F14" s="96"/>
@@ -3531,16 +3522,16 @@
     <row r="15" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="126"/>
       <c r="C15" s="97" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="98" t="s">
         <v>115</v>
-      </c>
-      <c r="F15" s="98" t="s">
-        <v>116</v>
       </c>
       <c r="G15" s="2">
         <v>44301</v>
@@ -3553,15 +3544,15 @@
     </row>
     <row r="16" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="126" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" s="12"/>
       <c r="E16" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" s="2">
         <v>44301</v>
@@ -3575,16 +3566,16 @@
     <row r="17" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="126"/>
       <c r="C17" s="101" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="98" t="s">
         <v>123</v>
-      </c>
-      <c r="F17" s="98" t="s">
-        <v>124</v>
       </c>
       <c r="G17" s="2">
         <v>44301</v>
@@ -3598,16 +3589,16 @@
     <row r="18" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="127"/>
       <c r="C18" s="102" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" s="103" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="103" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F18" s="104" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G18" s="2">
         <v>44301</v>
@@ -3623,7 +3614,7 @@
       <c r="C19" s="132"/>
       <c r="D19" s="133"/>
       <c r="E19" s="133" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F19" s="147"/>
       <c r="G19" s="2">
@@ -3640,7 +3631,7 @@
       <c r="C20" s="135"/>
       <c r="D20" s="136"/>
       <c r="E20" s="136" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F20" s="148"/>
       <c r="G20" s="153">
@@ -3684,12 +3675,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>I9=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:G19">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>I10=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3803,14 +3794,14 @@
     <row r="8" spans="3:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="49"/>
       <c r="F8" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I8" s="112" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J8" s="115"/>
       <c r="K8" s="116" t="s">
@@ -3828,11 +3819,11 @@
     <row r="9" spans="3:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="49"/>
       <c r="F9" s="105" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I9" s="106" t="s">
         <v>15</v>
@@ -3852,11 +3843,11 @@
       </c>
       <c r="D10" s="49"/>
       <c r="F10" s="105" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I10" s="111" t="s">
         <v>47</v>
@@ -3868,7 +3859,7 @@
         <v>18</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N10" s="38" t="s">
         <v>33</v>
@@ -3882,7 +3873,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I11" s="109" t="s">
         <v>0</v>
@@ -4094,8 +4085,8 @@
   </sheetPr>
   <dimension ref="C1:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4115,13 +4106,13 @@
     </row>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E2" s="59" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="F2" s="64" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I2" s="10"/>
       <c r="O2" s="12"/>
@@ -4132,10 +4123,10 @@
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F3" s="150" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G3" s="151" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I3" s="10"/>
       <c r="O3" s="152"/>
@@ -4149,7 +4140,7 @@
         <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O4" s="12"/>
       <c r="P4" s="154"/>
@@ -4174,10 +4165,10 @@
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E7" s="58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="154"/>
@@ -4187,7 +4178,7 @@
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F8" s="88" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
       <c r="G8" s="89"/>
       <c r="H8" s="60"/>
@@ -4204,7 +4195,7 @@
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F9" s="62" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -4224,10 +4215,10 @@
         <v>49</v>
       </c>
       <c r="G10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -4242,13 +4233,13 @@
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11" s="118" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="F11" s="62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -4264,25 +4255,25 @@
     </row>
     <row r="12" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="119" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="F12" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="H12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="J12" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="K12" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="55"/>
@@ -4294,28 +4285,28 @@
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F13" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="I13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="12" t="s">
+      <c r="K13" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="L13" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="M13" s="55" t="s">
         <v>68</v>
-      </c>
-      <c r="M13" s="55" t="s">
-        <v>69</v>
       </c>
       <c r="P13" s="154"/>
       <c r="Q13" s="154"/>
@@ -4324,10 +4315,10 @@
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F14" s="62" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -4342,10 +4333,10 @@
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F15" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -4356,10 +4347,10 @@
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F16" s="63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" s="72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="61"/>
       <c r="I16" s="61"/>
@@ -4373,16 +4364,16 @@
     </row>
     <row r="19" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E19" s="73" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F19" s="88" t="s">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="G19" s="89"/>
     </row>
     <row r="20" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F20" s="52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="60">
         <v>20</v>
@@ -4391,7 +4382,7 @@
         <v>25</v>
       </c>
       <c r="I20" s="69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="5:15" x14ac:dyDescent="0.25">
@@ -4399,33 +4390,33 @@
         <v>49</v>
       </c>
       <c r="G21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="I21" s="70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F22" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F23" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" s="61"/>
       <c r="H23" s="61"/>
       <c r="I23" s="71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
@@ -4433,53 +4424,53 @@
     </row>
     <row r="25" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E25" s="73" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F26" s="88" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
       <c r="G26" s="89"/>
       <c r="O26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F27" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" s="60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27" s="60"/>
       <c r="I27" s="53"/>
       <c r="K27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F28" s="67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="55"/>
       <c r="O28" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F29" s="67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="55"/>
       <c r="O29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="5:15" x14ac:dyDescent="0.25">
@@ -4488,66 +4479,66 @@
       <c r="H30" s="61"/>
       <c r="I30" s="57"/>
       <c r="O30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E32" s="74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F32" s="114" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G34" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I34" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G35" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I35" s="90" t="b">
         <v>1</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
@@ -4595,7 +4586,7 @@
         <v>30</v>
       </c>
       <c r="C1" s="92" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D1" s="92" t="s">
         <v>31</v>
@@ -4603,7 +4594,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4626,10 +4617,10 @@
   <sheetData>
     <row r="3" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="4:7" x14ac:dyDescent="0.25">
@@ -4640,29 +4631,29 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" t="s">
         <v>127</v>
       </c>
-      <c r="F5" t="s">
-        <v>128</v>
-      </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
@@ -4673,17 +4664,17 @@
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" t="str">
         <f>E5</f>
         <v>Read Bio</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4754,7 +4745,7 @@
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F12" s="1">
         <f ca="1">TODAY()</f>
-        <v>44292</v>
+        <v>44293</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
@@ -4764,7 +4755,7 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F12+90</f>
-        <v>44382</v>
+        <v>44383</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
@@ -4773,7 +4764,7 @@
       </c>
       <c r="F14" s="1">
         <f ca="1">F12+35</f>
-        <v>44327</v>
+        <v>44328</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added uuid for user table schema
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED5AC90-6D63-41C3-84C0-CEAC42596D06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7E1286-4D29-4646-8837-F6EF0AD70B0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30765" yWindow="975" windowWidth="22545" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="3810" yWindow="495" windowWidth="18900" windowHeight="15045" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="178">
   <si>
     <t>Questionaire</t>
   </si>
@@ -551,6 +551,24 @@
   </si>
   <si>
     <t>uername</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique id </t>
+  </si>
+  <si>
+    <t>Link Table</t>
+  </si>
+  <si>
+    <t>UUID</t>
+  </si>
+  <si>
+    <t>Profile ID</t>
+  </si>
+  <si>
+    <t>Pramaters ID</t>
   </si>
 </sst>
 </file>
@@ -750,7 +768,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -1414,6 +1432,21 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1421,7 +1454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1697,7 +1730,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1780,6 +1812,11 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3294,79 +3331,79 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="128" t="s">
+      <c r="D4" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="E4" s="128" t="s">
+      <c r="E4" s="127" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="128" t="s">
+      <c r="F4" s="127" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D5" s="128" t="s">
+      <c r="D5" s="127" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128" t="s">
+      <c r="E5" s="127"/>
+      <c r="F5" s="127" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="141"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="143" t="s">
+      <c r="B6" s="140"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="142" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="143" t="s">
+      <c r="E6" s="142" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="143" t="s">
+      <c r="F6" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="143" t="s">
+      <c r="G6" s="142" t="s">
         <v>150</v>
       </c>
-      <c r="H6" s="144" t="s">
+      <c r="H6" s="143" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="137" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="129" t="s">
+      <c r="C7" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="129" t="s">
+      <c r="D7" s="128" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="129" t="s">
+      <c r="E7" s="128" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="145" t="s">
+      <c r="F7" s="144" t="s">
         <v>94</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="137" t="s">
+      <c r="H7" s="136" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="139"/>
-      <c r="C8" s="129" t="s">
+      <c r="B8" s="138"/>
+      <c r="C8" s="128" t="s">
         <v>157</v>
       </c>
-      <c r="D8" s="130"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="157">
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="156">
         <v>44287</v>
       </c>
-      <c r="H8" s="156">
+      <c r="H8" s="155">
         <v>44287</v>
       </c>
       <c r="I8">
@@ -3374,11 +3411,11 @@
       </c>
       <c r="J8" s="1">
         <f ca="1">TODAY()</f>
-        <v>44293</v>
+        <v>44294</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="119" t="s">
         <v>111</v>
       </c>
       <c r="C9" s="91" t="s">
@@ -3393,10 +3430,10 @@
       <c r="F9" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="157">
+      <c r="G9" s="156">
         <v>44292</v>
       </c>
-      <c r="H9" s="156">
+      <c r="H9" s="155">
         <v>44292</v>
       </c>
       <c r="I9">
@@ -3405,7 +3442,7 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="121"/>
+      <c r="B10" s="120"/>
       <c r="C10" s="77" t="s">
         <v>91</v>
       </c>
@@ -3418,10 +3455,10 @@
       <c r="F10" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="157">
+      <c r="G10" s="156">
         <v>44292</v>
       </c>
-      <c r="H10" s="156">
+      <c r="H10" s="155">
         <v>44292</v>
       </c>
       <c r="I10">
@@ -3430,7 +3467,7 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="122"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="81" t="s">
         <v>100</v>
       </c>
@@ -3453,7 +3490,7 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="122" t="s">
         <v>110</v>
       </c>
       <c r="C12" s="83" t="s">
@@ -3478,7 +3515,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="124"/>
+      <c r="B13" s="123"/>
       <c r="C13" s="85" t="s">
         <v>108</v>
       </c>
@@ -3501,7 +3538,7 @@
       </c>
     </row>
     <row r="14" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="125"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="93" t="s">
         <v>112</v>
       </c>
@@ -3520,7 +3557,7 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="126"/>
+      <c r="B15" s="125"/>
       <c r="C15" s="97" t="s">
         <v>116</v>
       </c>
@@ -3543,7 +3580,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="126" t="s">
+      <c r="B16" s="125" t="s">
         <v>138</v>
       </c>
       <c r="C16" s="99"/>
@@ -3564,7 +3601,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="126"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="101" t="s">
         <v>116</v>
       </c>
@@ -3587,7 +3624,7 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="127"/>
+      <c r="B18" s="126"/>
       <c r="C18" s="102" t="s">
         <v>116</v>
       </c>
@@ -3610,34 +3647,34 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="131"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="133" t="s">
+      <c r="B19" s="130"/>
+      <c r="C19" s="131"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132" t="s">
         <v>158</v>
       </c>
-      <c r="F19" s="147"/>
+      <c r="F19" s="146"/>
       <c r="G19" s="2">
         <v>44303</v>
       </c>
-      <c r="H19" s="140"/>
+      <c r="H19" s="139"/>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="134"/>
-      <c r="C20" s="135"/>
-      <c r="D20" s="136"/>
-      <c r="E20" s="136" t="s">
+      <c r="B20" s="133"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="135" t="s">
         <v>159</v>
       </c>
-      <c r="F20" s="148"/>
-      <c r="G20" s="153">
+      <c r="F20" s="147"/>
+      <c r="G20" s="152">
         <v>44306</v>
       </c>
-      <c r="H20" s="149"/>
+      <c r="H20" s="148"/>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
@@ -4085,13 +4122,13 @@
   </sheetPr>
   <dimension ref="C1:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -4116,24 +4153,24 @@
       </c>
       <c r="I2" s="10"/>
       <c r="O2" s="12"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="154"/>
-      <c r="S2" s="154"/>
+      <c r="P2" s="153"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+      <c r="S2" s="153"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="F3" s="150" t="s">
+      <c r="F3" s="149" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="151" t="s">
+      <c r="G3" s="150" t="s">
         <v>164</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="O3" s="152"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="154"/>
-      <c r="R3" s="154"/>
-      <c r="S3" s="154"/>
+      <c r="O3" s="151"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="153"/>
+      <c r="R3" s="153"/>
+      <c r="S3" s="153"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F4" s="65" t="s">
@@ -4143,25 +4180,25 @@
         <v>165</v>
       </c>
       <c r="O4" s="12"/>
-      <c r="P4" s="154"/>
-      <c r="Q4" s="154"/>
-      <c r="R4" s="154"/>
-      <c r="S4" s="154"/>
+      <c r="P4" s="153"/>
+      <c r="Q4" s="153"/>
+      <c r="R4" s="153"/>
+      <c r="S4" s="153"/>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E5" s="34"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="154"/>
-      <c r="Q5" s="154"/>
-      <c r="R5" s="154"/>
-      <c r="S5" s="154"/>
+      <c r="P5" s="153"/>
+      <c r="Q5" s="153"/>
+      <c r="R5" s="153"/>
+      <c r="S5" s="153"/>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="O6" s="12"/>
-      <c r="P6" s="154"/>
-      <c r="Q6" s="154"/>
-      <c r="R6" s="154"/>
-      <c r="S6" s="154"/>
+      <c r="P6" s="153"/>
+      <c r="Q6" s="153"/>
+      <c r="R6" s="153"/>
+      <c r="S6" s="153"/>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E7" s="58" t="s">
@@ -4171,16 +4208,18 @@
         <v>136</v>
       </c>
       <c r="O7" s="12"/>
-      <c r="P7" s="154"/>
-      <c r="Q7" s="154"/>
-      <c r="R7" s="154"/>
-      <c r="S7" s="154"/>
+      <c r="P7" s="153"/>
+      <c r="Q7" s="153"/>
+      <c r="R7" s="153"/>
+      <c r="S7" s="153"/>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F8" s="88" t="s">
         <v>170</v>
       </c>
-      <c r="G8" s="89"/>
+      <c r="G8" s="89" t="s">
+        <v>173</v>
+      </c>
       <c r="H8" s="60"/>
       <c r="I8" s="60"/>
       <c r="J8" s="60"/>
@@ -4188,10 +4227,10 @@
       <c r="L8" s="60"/>
       <c r="M8" s="53"/>
       <c r="O8" s="12"/>
-      <c r="P8" s="154"/>
-      <c r="Q8" s="154"/>
-      <c r="R8" s="154"/>
-      <c r="S8" s="154"/>
+      <c r="P8" s="153"/>
+      <c r="Q8" s="153"/>
+      <c r="R8" s="153"/>
+      <c r="S8" s="153"/>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F9" s="62" t="s">
@@ -4205,10 +4244,10 @@
       <c r="L9" s="12"/>
       <c r="M9" s="55"/>
       <c r="O9" s="12"/>
-      <c r="P9" s="154"/>
-      <c r="Q9" s="154"/>
-      <c r="R9" s="154"/>
-      <c r="S9" s="154"/>
+      <c r="P9" s="153"/>
+      <c r="Q9" s="153"/>
+      <c r="R9" s="153"/>
+      <c r="S9" s="153"/>
     </row>
     <row r="10" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="62" t="s">
@@ -4226,10 +4265,10 @@
       <c r="L10" s="12"/>
       <c r="M10" s="55"/>
       <c r="O10" s="12"/>
-      <c r="P10" s="154"/>
-      <c r="Q10" s="154"/>
-      <c r="R10" s="154"/>
-      <c r="S10" s="154"/>
+      <c r="P10" s="153"/>
+      <c r="Q10" s="153"/>
+      <c r="R10" s="153"/>
+      <c r="S10" s="153"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11" s="118" t="s">
@@ -4248,13 +4287,13 @@
       <c r="L11" s="12"/>
       <c r="M11" s="55"/>
       <c r="O11" s="12"/>
-      <c r="P11" s="154"/>
-      <c r="Q11" s="154"/>
-      <c r="R11" s="154"/>
-      <c r="S11" s="154"/>
-    </row>
-    <row r="12" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="119" t="s">
+      <c r="P11" s="153"/>
+      <c r="Q11" s="153"/>
+      <c r="R11" s="153"/>
+      <c r="S11" s="153"/>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C12" s="160" t="s">
         <v>170</v>
       </c>
       <c r="F12" s="62" t="s">
@@ -4278,12 +4317,15 @@
       <c r="L12" s="12"/>
       <c r="M12" s="55"/>
       <c r="O12" s="12"/>
-      <c r="P12" s="154"/>
-      <c r="Q12" s="154"/>
-      <c r="R12" s="154"/>
-      <c r="S12" s="154"/>
+      <c r="P12" s="153"/>
+      <c r="Q12" s="153"/>
+      <c r="R12" s="153"/>
+      <c r="S12" s="153"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C13" s="161" t="s">
+        <v>172</v>
+      </c>
       <c r="F13" s="62" t="s">
         <v>61</v>
       </c>
@@ -4308,10 +4350,10 @@
       <c r="M13" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="P13" s="154"/>
-      <c r="Q13" s="154"/>
-      <c r="R13" s="154"/>
-      <c r="S13" s="154"/>
+      <c r="P13" s="153"/>
+      <c r="Q13" s="153"/>
+      <c r="R13" s="153"/>
+      <c r="S13" s="153"/>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F14" s="62" t="s">
@@ -4326,12 +4368,15 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="55"/>
-      <c r="P14" s="154"/>
-      <c r="Q14" s="154"/>
-      <c r="R14" s="154"/>
-      <c r="S14" s="154"/>
+      <c r="P14" s="153"/>
+      <c r="Q14" s="153"/>
+      <c r="R14" s="153"/>
+      <c r="S14" s="153"/>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="157" t="s">
+        <v>174</v>
+      </c>
       <c r="F15" s="62" t="s">
         <v>117</v>
       </c>
@@ -4346,6 +4391,9 @@
       <c r="M15" s="55"/>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C16" s="158" t="s">
+        <v>175</v>
+      </c>
       <c r="F16" s="63" t="s">
         <v>81</v>
       </c>
@@ -4359,10 +4407,19 @@
       <c r="L16" s="61"/>
       <c r="M16" s="57"/>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="158" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="158" t="s">
+        <v>177</v>
+      </c>
       <c r="E18" s="50"/>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="158"/>
       <c r="E19" s="73" t="s">
         <v>144</v>
       </c>
@@ -4371,7 +4428,8 @@
       </c>
       <c r="G19" s="89"/>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="158"/>
       <c r="F20" s="52" t="s">
         <v>56</v>
       </c>
@@ -4385,7 +4443,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="159"/>
       <c r="F21" s="54" t="s">
         <v>49</v>
       </c>
@@ -4399,7 +4458,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F22" s="54" t="s">
         <v>71</v>
       </c>
@@ -4409,7 +4468,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F23" s="56" t="s">
         <v>72</v>
       </c>
@@ -4419,15 +4478,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F24" s="34"/>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E25" s="73" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F26" s="88" t="s">
         <v>170</v>
       </c>
@@ -4436,7 +4495,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F27" s="66" t="s">
         <v>74</v>
       </c>
@@ -4449,7 +4508,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F28" s="67" t="s">
         <v>75</v>
       </c>
@@ -4462,7 +4521,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F29" s="67" t="s">
         <v>76</v>
       </c>
@@ -4473,7 +4532,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F30" s="68"/>
       <c r="G30" s="61"/>
       <c r="H30" s="61"/>
@@ -4482,7 +4541,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E32" s="74" t="s">
         <v>146</v>
       </c>
@@ -4745,7 +4804,7 @@
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F12" s="1">
         <f ca="1">TODAY()</f>
-        <v>44293</v>
+        <v>44294</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
@@ -4755,7 +4814,7 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F12+90</f>
-        <v>44383</v>
+        <v>44384</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
@@ -4764,7 +4823,7 @@
       </c>
       <c r="F14" s="1">
         <f ca="1">F12+35</f>
-        <v>44328</v>
+        <v>44329</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added api usename object button call to test and use for further development
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7E1286-4D29-4646-8837-F6EF0AD70B0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9860E866-95EE-43CB-8C85-3EE164F5FBE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="495" windowWidth="18900" windowHeight="15045" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="7260" yWindow="690" windowWidth="18255" windowHeight="14550" activeTab="6" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
     <sheet name="Overview" sheetId="2" r:id="rId2"/>
-    <sheet name="Database" sheetId="3" r:id="rId3"/>
-    <sheet name="Profile" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
+    <sheet name="User Path" sheetId="7" r:id="rId3"/>
+    <sheet name="Database" sheetId="3" r:id="rId4"/>
+    <sheet name="Profile" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Questions" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Database!$C$1:$R$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Database!$C$1:$R$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Overview!$C$3:$P$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Plan!$B$1:$H$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Questions!$E$1:$I$11</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="201">
   <si>
     <t>Questionaire</t>
   </si>
@@ -550,15 +552,9 @@
     <t>username</t>
   </si>
   <si>
-    <t>uername</t>
-  </si>
-  <si>
     <t>uuid</t>
   </si>
   <si>
-    <t xml:space="preserve">unique id </t>
-  </si>
-  <si>
     <t>Link Table</t>
   </si>
   <si>
@@ -569,6 +565,81 @@
   </si>
   <si>
     <t>Pramaters ID</t>
+  </si>
+  <si>
+    <t>My educational path has really helped me in life</t>
+  </si>
+  <si>
+    <t>In a party I love being the center of all attention</t>
+  </si>
+  <si>
+    <t>I deeply believe in religious expression/freedom</t>
+  </si>
+  <si>
+    <t>Happiness in life is more important then success</t>
+  </si>
+  <si>
+    <t>With my loved one I can live anywhere in the world</t>
+  </si>
+  <si>
+    <t>I adore children and would love to have my own</t>
+  </si>
+  <si>
+    <t>I love to work out daily for hours</t>
+  </si>
+  <si>
+    <t>I love to live in my dream world with sunshine and flowers</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>USER New</t>
+  </si>
+  <si>
+    <t>USER Old</t>
+  </si>
+  <si>
+    <t>Login/Signup</t>
+  </si>
+  <si>
+    <t>API Call USER</t>
+  </si>
+  <si>
+    <t>1. Logic to check if UUID (unique) exists</t>
+  </si>
+  <si>
+    <t>Profile complete</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Matched Page</t>
+  </si>
+  <si>
+    <t>To do Task</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>We are master of our own destiny</t>
+  </si>
+  <si>
+    <t>I love to be outdoors</t>
+  </si>
+  <si>
+    <t>This sits in logic Flow</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>num</t>
   </si>
 </sst>
 </file>
@@ -664,7 +735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -767,6 +838,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="62">
     <border>
@@ -1454,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1817,6 +1900,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2631,6 +2726,223 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30FC5392-B03E-406D-A975-A24CB33845BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2914650" y="2114550"/>
+          <a:ext cx="0" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776E9114-BEEF-4DE0-8FBC-9AEE0D6F4BC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2438400" y="3295650"/>
+          <a:ext cx="504825" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6FD95B3-B0C0-40AE-8772-D44421E676E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2952750" y="3333750"/>
+          <a:ext cx="361950" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2DFACF-DA3A-461D-AE3F-CD68225C6685}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3895725" y="2552700"/>
+          <a:ext cx="857250" cy="1200150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>27</xdr:row>
@@ -2737,14 +3049,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -2761,8 +3073,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1943100" y="1457326"/>
-          <a:ext cx="1638300" cy="723899"/>
+          <a:off x="1866900" y="1457326"/>
+          <a:ext cx="1885950" cy="723899"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3734,7 +4046,7 @@
   <dimension ref="C3:Q26"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,14 +4428,152 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40E4EF7-24E1-413C-97AA-C6968AF53715}">
+  <dimension ref="D5:M24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="66"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="53"/>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D7" s="67"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="55"/>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D8" s="68"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="57"/>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H13" s="164" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="162" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="163" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B17D3A9-07FE-487B-90F9-ABA82D7BC820}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="C1:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4215,11 +4665,9 @@
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F8" s="88" t="s">
-        <v>170</v>
-      </c>
-      <c r="G8" s="89" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="G8" s="89"/>
       <c r="H8" s="60"/>
       <c r="I8" s="60"/>
       <c r="J8" s="60"/>
@@ -4324,7 +4772,7 @@
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13" s="161" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" s="62" t="s">
         <v>61</v>
@@ -4375,7 +4823,7 @@
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15" s="157" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F15" s="62" t="s">
         <v>117</v>
@@ -4392,7 +4840,7 @@
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" s="158" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F16" s="63" t="s">
         <v>81</v>
@@ -4409,12 +4857,12 @@
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="158" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="158" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E18" s="50"/>
     </row>
@@ -4488,7 +4936,7 @@
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F26" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G26" s="89"/>
       <c r="O26" t="s">
@@ -4546,7 +4994,7 @@
         <v>146</v>
       </c>
       <c r="F32" s="114" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
@@ -4626,7 +5074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CFFAAF-81CA-40A5-B8AB-14E374916712}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4661,12 +5109,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8DFCEE-061A-480D-B5C6-F2C62A41425F}">
   <dimension ref="D3:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4741,132 +5189,188 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E7D01C-CDDC-4069-BB2D-9B21D940A6DD}">
-  <dimension ref="C4:J24"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="E1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F4">
-        <v>222000</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F5">
-        <f>F4*0.01</f>
-        <v>2220</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F6">
-        <f>F4*0.04</f>
-        <v>8880</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F7">
-        <f>F4*0.05</f>
-        <v>11100</v>
-      </c>
-      <c r="J7">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J9">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J10">
-        <f>SUM(J7:J9)</f>
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>690000</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="1">
-        <f ca="1">TODAY()</f>
-        <v>44294</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <f>C11*0.04</f>
-        <v>27600</v>
-      </c>
-      <c r="F13" s="2">
-        <f ca="1">F12+90</f>
-        <v>44384</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14">
+    <row r="1" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E1" s="165" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="166" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="167" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="167" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="165">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="165">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E4" s="165">
         <v>3</v>
       </c>
-      <c r="F14" s="1">
-        <f ca="1">F12+35</f>
-        <v>44329</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J16">
-        <v>200.15</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J17">
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J18">
-        <f>J17+J16</f>
-        <v>1875.15</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20">
-        <v>222222</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f>F20*0.0275</f>
-        <v>6111.1050000000005</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23">
-        <f>F22*0.35</f>
-        <v>2138.8867500000001</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <f>F22-F23</f>
-        <v>3972.2182500000004</v>
-      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="165">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="165">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="165">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="165">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G8" t="s">
+        <v>200</v>
+      </c>
+      <c r="H8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="165">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="165">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" t="s">
+        <v>200</v>
+      </c>
+      <c r="H10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="165">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>197</v>
+      </c>
+      <c r="G11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added user api functionality  (#5)
* testing new githug organization

* added api usename object button call to test and use for further development
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7E1286-4D29-4646-8837-F6EF0AD70B0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9860E866-95EE-43CB-8C85-3EE164F5FBE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="495" windowWidth="18900" windowHeight="15045" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="7260" yWindow="690" windowWidth="18255" windowHeight="14550" activeTab="6" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
     <sheet name="Overview" sheetId="2" r:id="rId2"/>
-    <sheet name="Database" sheetId="3" r:id="rId3"/>
-    <sheet name="Profile" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
+    <sheet name="User Path" sheetId="7" r:id="rId3"/>
+    <sheet name="Database" sheetId="3" r:id="rId4"/>
+    <sheet name="Profile" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Questions" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Database!$C$1:$R$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Database!$C$1:$R$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Overview!$C$3:$P$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Plan!$B$1:$H$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Questions!$E$1:$I$11</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="201">
   <si>
     <t>Questionaire</t>
   </si>
@@ -550,15 +552,9 @@
     <t>username</t>
   </si>
   <si>
-    <t>uername</t>
-  </si>
-  <si>
     <t>uuid</t>
   </si>
   <si>
-    <t xml:space="preserve">unique id </t>
-  </si>
-  <si>
     <t>Link Table</t>
   </si>
   <si>
@@ -569,6 +565,81 @@
   </si>
   <si>
     <t>Pramaters ID</t>
+  </si>
+  <si>
+    <t>My educational path has really helped me in life</t>
+  </si>
+  <si>
+    <t>In a party I love being the center of all attention</t>
+  </si>
+  <si>
+    <t>I deeply believe in religious expression/freedom</t>
+  </si>
+  <si>
+    <t>Happiness in life is more important then success</t>
+  </si>
+  <si>
+    <t>With my loved one I can live anywhere in the world</t>
+  </si>
+  <si>
+    <t>I adore children and would love to have my own</t>
+  </si>
+  <si>
+    <t>I love to work out daily for hours</t>
+  </si>
+  <si>
+    <t>I love to live in my dream world with sunshine and flowers</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>USER New</t>
+  </si>
+  <si>
+    <t>USER Old</t>
+  </si>
+  <si>
+    <t>Login/Signup</t>
+  </si>
+  <si>
+    <t>API Call USER</t>
+  </si>
+  <si>
+    <t>1. Logic to check if UUID (unique) exists</t>
+  </si>
+  <si>
+    <t>Profile complete</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Matched Page</t>
+  </si>
+  <si>
+    <t>To do Task</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>We are master of our own destiny</t>
+  </si>
+  <si>
+    <t>I love to be outdoors</t>
+  </si>
+  <si>
+    <t>This sits in logic Flow</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>num</t>
   </si>
 </sst>
 </file>
@@ -664,7 +735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -767,6 +838,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="62">
     <border>
@@ -1454,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1817,6 +1900,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2631,6 +2726,223 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30FC5392-B03E-406D-A975-A24CB33845BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2914650" y="2114550"/>
+          <a:ext cx="0" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776E9114-BEEF-4DE0-8FBC-9AEE0D6F4BC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2438400" y="3295650"/>
+          <a:ext cx="504825" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6FD95B3-B0C0-40AE-8772-D44421E676E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2952750" y="3333750"/>
+          <a:ext cx="361950" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2DFACF-DA3A-461D-AE3F-CD68225C6685}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3895725" y="2552700"/>
+          <a:ext cx="857250" cy="1200150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>27</xdr:row>
@@ -2737,14 +3049,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -2761,8 +3073,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1943100" y="1457326"/>
-          <a:ext cx="1638300" cy="723899"/>
+          <a:off x="1866900" y="1457326"/>
+          <a:ext cx="1885950" cy="723899"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3734,7 +4046,7 @@
   <dimension ref="C3:Q26"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,14 +4428,152 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40E4EF7-24E1-413C-97AA-C6968AF53715}">
+  <dimension ref="D5:M24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="66"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="53"/>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D7" s="67"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="55"/>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D8" s="68"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="57"/>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H13" s="164" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="162" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="163" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B17D3A9-07FE-487B-90F9-ABA82D7BC820}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="C1:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4215,11 +4665,9 @@
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F8" s="88" t="s">
-        <v>170</v>
-      </c>
-      <c r="G8" s="89" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="G8" s="89"/>
       <c r="H8" s="60"/>
       <c r="I8" s="60"/>
       <c r="J8" s="60"/>
@@ -4324,7 +4772,7 @@
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13" s="161" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" s="62" t="s">
         <v>61</v>
@@ -4375,7 +4823,7 @@
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15" s="157" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F15" s="62" t="s">
         <v>117</v>
@@ -4392,7 +4840,7 @@
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" s="158" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F16" s="63" t="s">
         <v>81</v>
@@ -4409,12 +4857,12 @@
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="158" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="158" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E18" s="50"/>
     </row>
@@ -4488,7 +4936,7 @@
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F26" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G26" s="89"/>
       <c r="O26" t="s">
@@ -4546,7 +4994,7 @@
         <v>146</v>
       </c>
       <c r="F32" s="114" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
@@ -4626,7 +5074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CFFAAF-81CA-40A5-B8AB-14E374916712}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4661,12 +5109,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8DFCEE-061A-480D-B5C6-F2C62A41425F}">
   <dimension ref="D3:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4741,132 +5189,188 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E7D01C-CDDC-4069-BB2D-9B21D940A6DD}">
-  <dimension ref="C4:J24"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="E1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F4">
-        <v>222000</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F5">
-        <f>F4*0.01</f>
-        <v>2220</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F6">
-        <f>F4*0.04</f>
-        <v>8880</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F7">
-        <f>F4*0.05</f>
-        <v>11100</v>
-      </c>
-      <c r="J7">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J9">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J10">
-        <f>SUM(J7:J9)</f>
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>690000</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="1">
-        <f ca="1">TODAY()</f>
-        <v>44294</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <f>C11*0.04</f>
-        <v>27600</v>
-      </c>
-      <c r="F13" s="2">
-        <f ca="1">F12+90</f>
-        <v>44384</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14">
+    <row r="1" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E1" s="165" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="166" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="167" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="167" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="165">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="165">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E4" s="165">
         <v>3</v>
       </c>
-      <c r="F14" s="1">
-        <f ca="1">F12+35</f>
-        <v>44329</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J16">
-        <v>200.15</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J17">
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J18">
-        <f>J17+J16</f>
-        <v>1875.15</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20">
-        <v>222222</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f>F20*0.0275</f>
-        <v>6111.1050000000005</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23">
-        <f>F22*0.35</f>
-        <v>2138.8867500000001</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <f>F22-F23</f>
-        <v>3972.2182500000004</v>
-      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="165">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="165">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="165">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="165">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G8" t="s">
+        <v>200</v>
+      </c>
+      <c r="H8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="165">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="165">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" t="s">
+        <v>200</v>
+      </c>
+      <c r="H10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="165">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>197</v>
+      </c>
+      <c r="G11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>